<commit_message>
Updated VIN control table files to do not change MSRP version for new versions and use the correct one for each product
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/controlTable_CA_CHOICE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gu1xkaz\IdeaProjects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>PRODUCTCD</t>
   </si>
@@ -60,9 +60,6 @@
   </si>
   <si>
     <t>MSRP_2000_CHOICE</t>
-  </si>
-  <si>
-    <t>MSRP_2000_CHOICE_T</t>
   </si>
   <si>
     <t>MSRP_VERSION</t>
@@ -411,7 +408,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -490,7 +487,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>